<commit_message>
Add labels to spreadsheet with Mincer reg results
</commit_message>
<xml_diff>
--- a/data/Mincer.xlsx
+++ b/data/Mincer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\GitHub\teachers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5922D8A-C127-4DAA-8D0C-4E03DC9BDD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B7BAC1-8DC4-46F1-A0CD-A924A47394FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3531A8FF-D0DF-4403-A910-B6CFC06880B8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{3531A8FF-D0DF-4403-A910-B6CFC06880B8}"/>
   </bookViews>
   <sheets>
     <sheet name="mincer" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>ln (hourly wage in $1999)=const+b1*school+b2*age+b3*age^2+e</t>
   </si>
@@ -64,6 +64,66 @@
   </si>
   <si>
     <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>Executives, Administrative, and Managerial</t>
+  </si>
+  <si>
+    <t>Management Related</t>
+  </si>
+  <si>
+    <t>Architects, Engineers, Math, and Computer Science</t>
+  </si>
+  <si>
+    <t>Natural and Social Scientists, Recreation, Religious, Arts, Athletes</t>
+  </si>
+  <si>
+    <t>Doctors and Lawyers</t>
+  </si>
+  <si>
+    <t>Nurses, Therapists, and Other Health Service</t>
+  </si>
+  <si>
+    <t>Teachers, Postsecondary</t>
+  </si>
+  <si>
+    <t>Teachers, Non-Postsecondary and Librarians</t>
+  </si>
+  <si>
+    <t>Health and Science Technicians</t>
+  </si>
+  <si>
+    <t>Sales, All</t>
+  </si>
+  <si>
+    <t>Administrative Support, Clerks, Record</t>
+  </si>
+  <si>
+    <t>Fire, Police, and Guards</t>
+  </si>
+  <si>
+    <t>Food, Cleaning, and Personal Services and Private Household</t>
+  </si>
+  <si>
+    <t>Farm, Related Agrigulture, Logging, and Extraction</t>
+  </si>
+  <si>
+    <t>Mechanics and Construction</t>
+  </si>
+  <si>
+    <t>Precision Manufacturing</t>
+  </si>
+  <si>
+    <t>Manufacturing Operators</t>
+  </si>
+  <si>
+    <t>Fabricators, Inspectors, and Material Handlers</t>
+  </si>
+  <si>
+    <t>Vehicle Operators</t>
+  </si>
+  <si>
+    <t>Kindergarten - Secondary Teachers</t>
   </si>
 </sst>
 </file>
@@ -71,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -102,13 +162,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C199A06F-B415-4E41-A46B-FF2F420B5050}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -468,53 +527,53 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>4.4667600000000002E-2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>5.3321199999999999E-2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>4.90593E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>8.25322E-2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>8.9569899999999994E-2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>0.10256319999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>3.9692031906802254E-2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>4.7471048681422184E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>4.5976864536856045E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>7.7059687667519472E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>8.2138246754080921E-2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <v>9.6556296030251135E-2</v>
       </c>
     </row>
@@ -522,22 +581,22 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>3.7630682204947377E-2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>4.409366478932937E-2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>4.0162686188585865E-2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>6.8209358946771853E-2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>7.2688045151711525E-2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <v>8.3074437174163407E-2</v>
       </c>
     </row>
@@ -545,22 +604,22 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>4.7699135102262057E-2</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>5.8395997008662423E-2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>5.6754782376008638E-2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>8.9878162009358498E-2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>9.4996393622356748E-2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="1">
         <v>0.11229458258696567</v>
       </c>
     </row>
@@ -573,44 +632,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C36A22-EAE7-42E3-8116-80C5DAB13E2F}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>1960</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2">
         <v>1970</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2">
         <v>1980</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2">
         <v>1990</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2">
         <v>2000</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2">
         <v>2010</v>
       </c>
-      <c r="M1" s="1"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>7.0900000000000005E-2</v>
@@ -650,8 +712,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
         <v>3.9800000000000002E-2</v>
@@ -691,8 +753,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4">
         <v>4.9099999999999998E-2</v>
@@ -732,8 +794,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
       <c r="B5">
         <v>-1.38E-2</v>
@@ -773,8 +835,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>13</v>
       </c>
       <c r="B6">
         <v>1.55E-2</v>
@@ -814,8 +876,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>14</v>
       </c>
       <c r="B7">
         <v>9.9500000000000005E-2</v>
@@ -855,8 +917,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>15</v>
       </c>
       <c r="B8">
         <v>2.46E-2</v>
@@ -896,8 +958,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
       <c r="B9">
         <v>2.4500000000000001E-2</v>
@@ -937,8 +999,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>17</v>
       </c>
       <c r="B10">
         <v>1.84E-2</v>
@@ -978,8 +1040,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>18</v>
       </c>
       <c r="B11">
         <v>6.5799999999999997E-2</v>
@@ -1019,8 +1081,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>19</v>
       </c>
       <c r="B12">
         <v>2.6700000000000002E-2</v>
@@ -1060,8 +1122,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>20</v>
       </c>
       <c r="B13">
         <v>3.2500000000000001E-2</v>
@@ -1101,8 +1163,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>21</v>
       </c>
       <c r="B14">
         <v>1.23E-2</v>
@@ -1142,8 +1204,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>22</v>
       </c>
       <c r="B15">
         <v>4.4400000000000002E-2</v>
@@ -1183,8 +1245,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>23</v>
       </c>
       <c r="B16">
         <v>2.93E-2</v>
@@ -1224,8 +1286,8 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>24</v>
       </c>
       <c r="B17">
         <v>3.7400000000000003E-2</v>
@@ -1265,8 +1327,8 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>25</v>
       </c>
       <c r="B18">
         <v>4.6300000000000001E-2</v>
@@ -1306,8 +1368,8 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>26</v>
       </c>
       <c r="B19">
         <v>2.3599999999999999E-2</v>
@@ -1347,8 +1409,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>27</v>
       </c>
       <c r="B20">
         <v>1.8800000000000001E-2</v>
@@ -1388,8 +1450,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>100</v>
+      <c r="A21" t="s">
+        <v>28</v>
       </c>
       <c r="B21">
         <v>2.76E-2</v>
@@ -1485,848 +1547,848 @@
       <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>1960</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
         <v>1970</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
         <v>1980</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2">
         <v>1990</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2">
         <v>2000</v>
       </c>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1">
+      <c r="K25" s="2"/>
+      <c r="L25" s="2">
         <v>2010</v>
       </c>
-      <c r="M25" s="1"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
+      <c r="A26" t="s">
+        <v>9</v>
       </c>
       <c r="B26">
         <v>9.8500000000000004E-2</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>2322</v>
       </c>
       <c r="D26">
         <v>8.1299999999999997E-2</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>1829</v>
       </c>
       <c r="F26">
         <v>7.0199999999999999E-2</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26">
         <v>23238</v>
       </c>
       <c r="H26">
         <v>9.5100000000000004E-2</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26">
         <v>46673</v>
       </c>
       <c r="J26">
         <v>0.10299999999999999</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26">
         <v>39543</v>
       </c>
       <c r="L26">
         <v>0.113</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26">
         <v>44932</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2</v>
+      <c r="A27" t="s">
+        <v>10</v>
       </c>
       <c r="B27">
         <v>4.4400000000000002E-2</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>873</v>
       </c>
       <c r="D27">
         <v>8.09E-2</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>643</v>
       </c>
       <c r="F27">
         <v>6.3200000000000006E-2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27">
         <v>13893</v>
       </c>
       <c r="H27">
         <v>9.2100000000000001E-2</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27">
         <v>26556</v>
       </c>
       <c r="J27">
         <v>9.2100000000000001E-2</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27">
         <v>27794</v>
       </c>
       <c r="L27">
         <v>0.107</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27">
         <v>28486</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3</v>
+      <c r="A28" t="s">
+        <v>11</v>
       </c>
       <c r="B28">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>157</v>
       </c>
       <c r="D28">
         <v>7.8299999999999995E-2</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28">
         <v>245</v>
       </c>
       <c r="F28">
         <v>5.9900000000000002E-2</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28">
         <v>2952</v>
       </c>
       <c r="H28">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28">
         <v>8208</v>
       </c>
       <c r="J28">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28">
         <v>9642</v>
       </c>
       <c r="L28">
         <v>0.123</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28">
         <v>9787</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>4</v>
+      <c r="A29" t="s">
+        <v>12</v>
       </c>
       <c r="B29">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>1668</v>
       </c>
       <c r="D29">
         <v>9.7799999999999998E-2</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>1277</v>
       </c>
       <c r="F29">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29">
         <v>11592</v>
       </c>
       <c r="H29">
         <v>8.9899999999999994E-2</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29">
         <v>17275</v>
       </c>
       <c r="J29">
         <v>8.4599999999999995E-2</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29">
         <v>18849</v>
       </c>
       <c r="L29">
         <v>9.8900000000000002E-2</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29">
         <v>24365</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="B30" s="2">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>204</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
         <v>5.16E-2</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>138</v>
       </c>
       <c r="F30">
         <v>9.1800000000000007E-2</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30">
         <v>2457</v>
       </c>
       <c r="H30">
         <v>0.19</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30">
         <v>4761</v>
       </c>
       <c r="J30">
         <v>4.7600000000000003E-2</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30">
         <v>5690</v>
       </c>
       <c r="L30">
         <v>3.9899999999999998E-2</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30">
         <v>8845</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>6</v>
+      <c r="A31" t="s">
+        <v>14</v>
       </c>
       <c r="B31">
         <v>9.1800000000000007E-2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>5290</v>
       </c>
       <c r="D31">
         <v>0.11899999999999999</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>3475</v>
       </c>
       <c r="F31">
         <v>0.11600000000000001</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31">
         <v>26534</v>
       </c>
       <c r="H31">
         <v>0.17899999999999999</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31">
         <v>37891</v>
       </c>
       <c r="J31">
         <v>0.16500000000000001</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31">
         <v>40085</v>
       </c>
       <c r="L31">
         <v>0.19500000000000001</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31">
         <v>60037</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>7</v>
-      </c>
-      <c r="B32" s="2">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32">
         <v>8.0399999999999999E-2</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>92</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32">
         <v>6.5299999999999997E-2</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>184</v>
       </c>
       <c r="F32">
         <v>6.6900000000000001E-2</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32">
         <v>1268</v>
       </c>
       <c r="H32">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32">
         <v>1156</v>
       </c>
       <c r="J32">
         <v>2.7699999999999999E-2</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32">
         <v>2247</v>
       </c>
       <c r="L32">
         <v>6.0299999999999999E-2</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32">
         <v>4239</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>8</v>
+      <c r="A33" t="s">
+        <v>16</v>
       </c>
       <c r="B33">
         <v>9.2200000000000004E-2</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>287</v>
       </c>
       <c r="D33">
         <v>0.18099999999999999</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33">
         <v>267</v>
       </c>
       <c r="F33">
         <v>0.122</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33">
         <v>2307</v>
       </c>
       <c r="H33">
         <v>0.158</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33">
         <v>3623</v>
       </c>
       <c r="J33">
         <v>0.123</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33">
         <v>5703</v>
       </c>
       <c r="L33">
         <v>0.13900000000000001</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33">
         <v>8960</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>9</v>
+      <c r="A34" t="s">
+        <v>17</v>
       </c>
       <c r="B34">
         <v>8.2199999999999995E-2</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>2183</v>
       </c>
       <c r="D34">
         <v>7.4499999999999997E-2</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34">
         <v>2316</v>
       </c>
       <c r="F34">
         <v>6.8400000000000002E-2</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34">
         <v>15906</v>
       </c>
       <c r="H34">
         <v>9.5600000000000004E-2</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34">
         <v>24626</v>
       </c>
       <c r="J34">
         <v>0.108</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34">
         <v>21460</v>
       </c>
       <c r="L34">
         <v>0.104</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34">
         <v>22118</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>10</v>
+      <c r="A35" t="s">
+        <v>18</v>
       </c>
       <c r="B35">
         <v>6.9599999999999995E-2</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>4419</v>
       </c>
       <c r="D35">
         <v>6.9800000000000001E-2</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35">
         <v>2644</v>
       </c>
       <c r="F35">
         <v>7.7799999999999994E-2</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35">
         <v>22339</v>
       </c>
       <c r="H35">
         <v>0.13600000000000001</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35">
         <v>45680</v>
       </c>
       <c r="J35">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35">
         <v>43756</v>
       </c>
       <c r="L35">
         <v>0.13800000000000001</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M35">
         <v>42370</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>11</v>
+      <c r="A36" t="s">
+        <v>19</v>
       </c>
       <c r="B36">
         <v>3.1699999999999999E-2</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>38055</v>
       </c>
       <c r="D36">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36">
         <v>21116</v>
       </c>
       <c r="F36">
         <v>3.1099999999999999E-2</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36">
         <v>118586</v>
       </c>
       <c r="H36">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36">
         <v>136018</v>
       </c>
       <c r="J36">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36">
         <v>114529</v>
       </c>
       <c r="L36">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36">
         <v>92826</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>12</v>
+      <c r="A37" t="s">
+        <v>20</v>
       </c>
       <c r="B37">
         <v>9.6500000000000002E-2</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37">
         <v>79</v>
       </c>
       <c r="D37">
         <v>0.113</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>79</v>
       </c>
       <c r="F37">
         <v>8.5699999999999998E-2</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37">
         <v>1317</v>
       </c>
       <c r="H37">
         <v>8.2100000000000006E-2</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37">
         <v>3397</v>
       </c>
       <c r="J37">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37">
         <v>4983</v>
       </c>
       <c r="L37">
         <v>9.0200000000000002E-2</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37">
         <v>5479</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>13</v>
+      <c r="A38" t="s">
+        <v>21</v>
       </c>
       <c r="B38">
         <v>6.0400000000000002E-2</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38">
         <v>6511</v>
       </c>
       <c r="D38">
         <v>6.4199999999999993E-2</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38">
         <v>4116</v>
       </c>
       <c r="F38">
         <v>3.7400000000000003E-2</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38">
         <v>18817</v>
       </c>
       <c r="H38">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38">
         <v>33633</v>
       </c>
       <c r="J38">
         <v>7.1499999999999994E-2</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38">
         <v>36991</v>
       </c>
       <c r="L38">
         <v>6.93E-2</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38">
         <v>40793</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>14</v>
-      </c>
-      <c r="B39" s="2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
         <v>2.3199999999999998E-2</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39">
         <v>156</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39">
         <v>7.6100000000000001E-2</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39">
         <v>159</v>
       </c>
       <c r="F39">
         <v>2.7300000000000001E-2</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39">
         <v>1530</v>
       </c>
       <c r="H39">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39">
         <v>2863</v>
       </c>
       <c r="J39">
         <v>3.9199999999999999E-2</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39">
         <v>2217</v>
       </c>
       <c r="L39">
         <v>5.5199999999999999E-2</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39">
         <v>2646</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>15</v>
-      </c>
-      <c r="B40" s="2">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40">
         <v>-6.4799999999999996E-3</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>204</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40">
         <v>2.46E-2</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40">
         <v>331</v>
       </c>
       <c r="F40">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40">
         <v>2470</v>
       </c>
       <c r="H40">
         <v>7.6300000000000007E-2</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40">
         <v>3884</v>
       </c>
       <c r="J40">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40">
         <v>3504</v>
       </c>
       <c r="L40">
         <v>6.3E-2</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40">
         <v>2016</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>16</v>
+      <c r="A41" t="s">
+        <v>24</v>
       </c>
       <c r="B41">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>654</v>
       </c>
       <c r="D41">
         <v>5.5399999999999998E-2</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>612</v>
       </c>
       <c r="F41">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41">
         <v>5214</v>
       </c>
       <c r="H41">
         <v>9.1700000000000004E-2</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41">
         <v>7421</v>
       </c>
       <c r="J41">
         <v>8.8599999999999998E-2</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41">
         <v>5546</v>
       </c>
       <c r="L41">
         <v>8.9399999999999993E-2</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41">
         <v>3371</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>17</v>
+      <c r="A42" t="s">
+        <v>25</v>
       </c>
       <c r="B42">
         <v>2.41E-2</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>7866</v>
       </c>
       <c r="D42">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42">
         <v>4484</v>
       </c>
       <c r="F42">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42">
         <v>14961</v>
       </c>
       <c r="H42">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42">
         <v>17595</v>
       </c>
       <c r="J42">
         <v>7.3200000000000001E-2</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42">
         <v>11385</v>
       </c>
       <c r="L42">
         <v>8.7900000000000006E-2</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42">
         <v>4749</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>18</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43">
         <v>1.11E-2</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43">
         <v>2231</v>
       </c>
       <c r="D43">
         <v>1.8800000000000001E-2</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43">
         <v>1988</v>
       </c>
       <c r="F43">
         <v>3.5499999999999997E-2</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43">
         <v>13972</v>
       </c>
       <c r="H43">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43">
         <v>18141</v>
       </c>
       <c r="J43">
         <v>7.5200000000000003E-2</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43">
         <v>12350</v>
       </c>
       <c r="L43">
         <v>9.4600000000000004E-2</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M43">
         <v>6584</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>19</v>
+      <c r="A44" t="s">
+        <v>27</v>
       </c>
       <c r="B44">
         <v>7.3700000000000002E-2</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44">
         <v>99</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44">
         <v>-1.21E-2</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44">
         <v>107</v>
       </c>
       <c r="F44">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44">
         <v>1573</v>
       </c>
       <c r="H44">
         <v>8.1699999999999995E-2</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44">
         <v>3090</v>
       </c>
       <c r="J44">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44">
         <v>3106</v>
       </c>
       <c r="L44">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44">
         <v>2122</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>100</v>
+      <c r="A45" t="s">
+        <v>28</v>
       </c>
       <c r="B45">
         <v>0.151</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45">
         <v>2289</v>
       </c>
       <c r="D45">
         <v>0.11</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45">
         <v>2129</v>
       </c>
       <c r="F45">
         <v>0.11899999999999999</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45">
         <v>12987</v>
       </c>
       <c r="H45">
         <v>0.14799999999999999</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45">
         <v>13137</v>
       </c>
       <c r="J45">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45">
         <v>19305</v>
       </c>
       <c r="L45">
         <v>0.16</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45">
         <v>37465</v>
       </c>
     </row>
@@ -2392,7 +2454,7 @@
         <v>3.9692031906802254E-2</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="C48:M48" si="0">(D22*E22+D46*E46)/(E22+E46)</f>
+        <f t="shared" ref="D48:L48" si="0">(D22*E22+D46*E46)/(E22+E46)</f>
         <v>4.7471048681422184E-2</v>
       </c>
       <c r="F48">
@@ -2414,11 +2476,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -2426,6 +2483,11 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>